<commit_message>
Add Currency node to xml
</commit_message>
<xml_diff>
--- a/Data/OutputTableRows.xlsx
+++ b/Data/OutputTableRows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\libor\Dropbox\LK_docs\Valuetools\Zákazníci\Benet Automotive\Demo Process\Invoice-RossumDataExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F190330-EC83-4A35-B505-A8171EEBE4E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450DA26F-BFB3-4668-9FD5-B6BA49AA4B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2630" windowWidth="31220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4730" yWindow="850" windowWidth="31220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Variabilní symbol</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>BenetOrderNumber</t>
+  </si>
+  <si>
+    <t>Měna dokladu</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,117 +572,128 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added currency to xml Final
</commit_message>
<xml_diff>
--- a/Data/OutputTableRows.xlsx
+++ b/Data/OutputTableRows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\libor\Dropbox\LK_docs\Valuetools\Zákazníci\Benet Automotive\Demo Process\Invoice-RossumDataExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450DA26F-BFB3-4668-9FD5-B6BA49AA4B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B9C53-FB7A-47EE-B830-83E506058B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4730" yWindow="850" windowWidth="31220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="1040" windowWidth="31220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Final verion for Testing
</commit_message>
<xml_diff>
--- a/Data/OutputTableRows.xlsx
+++ b/Data/OutputTableRows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\libor\Dropbox\LK_docs\Valuetools\Zákazníci\Benet Automotive\Demo Process\Invoice-RossumDataExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B9C53-FB7A-47EE-B830-83E506058B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2631BE06-2C95-42CA-9D73-758A11E60A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="1040" windowWidth="31220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="33280" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Variabilní symbol</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Delivery Note</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,6 +648,9 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>